<commit_message>
updating heat pump model
</commit_message>
<xml_diff>
--- a/Data Scraping/Pump1.xlsx
+++ b/Data Scraping/Pump1.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11.9</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,9 @@
       <c r="P1" s="1" t="n">
         <v>14</v>
       </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -546,7 +549,7 @@
           <t>INDOOR</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>OUTDOOR TEMPERATURE (°CDB)</t>
         </is>
@@ -563,27 +566,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>20</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>25.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>30.0 32.0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>35.0</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>40.0</t>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>30 32</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>40</t>
         </is>
       </c>
     </row>
@@ -628,35 +631,45 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>TC SHC PI TC SHC PI</t>
+          <t>TC</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>SHC PI TC SHC</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>SHC</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>SHC</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
@@ -668,7 +681,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14.0 20</t>
+          <t>14.0 20.0</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -678,12 +691,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2.42</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -693,47 +706,57 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2.37</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2.46 2.31 0.52 2.41 2.29 0.54</t>
+          <t>2.46</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2.14 0.54 2.41 2.12</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>2.34</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>2.26</t>
-        </is>
-      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>2.08</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
+          <t>0.58</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
           <t>2.21</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2.20</t>
-        </is>
-      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>2.03</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -743,7 +766,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16.0 22</t>
+          <t>16.0 22.0</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -753,12 +776,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.38</t>
+          <t>2.21</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -768,47 +791,57 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>2.16</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2.58</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2.11 0.54 2.53 2.09</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2.46</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2.06</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
           <t>2.33</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0.48</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2.58 2.28 0.52 2.53 2.26 0.54</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2.46</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>2.23</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.57</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>2.33</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>2.18</t>
-        </is>
-      </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -818,7 +851,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18.0 25</t>
+          <t>18.0 25.0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -828,12 +861,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2.56</t>
+          <t>2.36</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -843,47 +876,57 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2.51</t>
+          <t>2.31</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2.70 2.46 0.53 2.65 2.44 0.54</t>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2.26 0.55 2.65 2.24</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>2.58</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>2.41</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>2.21</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
           <t>2.46</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2.37</t>
-        </is>
-      </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>2.16</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -903,12 +946,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.75</t>
+          <t>2.52</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -918,47 +961,57 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2.70</t>
+          <t>2.47</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2.76 2.66 0.53 2.71 2.64 0.54</t>
+          <t>2.76</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2.42 0.55 2.71 2.40</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
           <t>2.64</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>2.61</t>
-        </is>
-      </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>2.37</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
           <t>2.52</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>2.56</t>
-        </is>
-      </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0.60</t>
         </is>
       </c>
     </row>
@@ -968,7 +1021,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>22.0 30</t>
+          <t>22.0 30.0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -978,12 +1031,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.67</t>
+          <t>2.44</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -993,47 +1046,57 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2.63</t>
+          <t>2.40</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2.95 2.59 0.53 2.90 2.57 0.55</t>
+          <t>2.95</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2.35 0.55 2.90 2.34</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>2.82</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>2.55</t>
-        </is>
-      </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>2.31</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>2.70</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>2.51</t>
-        </is>
-      </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>0.60</t>
         </is>
       </c>
     </row>
@@ -1043,7 +1106,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24.0 32</t>
+          <t>24.0 32.0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1053,12 +1116,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.62</t>
+          <t>2.39</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.47</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1068,47 +1131,57 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2.58</t>
+          <t>2.35</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3.07 2.54 0.53 3.02 2.53 0.55</t>
+          <t>3.07</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2.31 0.55 3.02 2.29</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t>2.94</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>2.51</t>
-        </is>
-      </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>2.27</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
           <t>2.82</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>2.47</t>
-        </is>
-      </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0.60</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1196,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1177,6 +1250,9 @@
       <c r="P1" s="1" t="n">
         <v>14</v>
       </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1187,7 +1263,7 @@
           <t>INDOOR</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>OUTDOOR TEMPERATURE (°FDB)</t>
         </is>
@@ -1204,27 +1280,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>68.0</t>
+          <t>68</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>77.0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>86.0 89.6</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>95.0</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>104.0</t>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>86 90</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>104</t>
         </is>
       </c>
     </row>
@@ -1269,35 +1345,45 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>TC SHC PI TC SHC PI</t>
+          <t>TC</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>SHC PI TC SHC</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>SHC</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>SHC</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
@@ -1319,12 +1405,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>8.27</t>
+          <t>7.68</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1334,47 +1420,57 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>8.08</t>
+          <t>7.49</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>8.39 7.89 0.52 8.22 7.81 0.54</t>
+          <t>8.39</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>7.29 0.54 8.22 7.22</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>7.97</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>7.70</t>
-        </is>
-      </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>7.10</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
+          <t>0.58</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
           <t>7.55</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>7.52</t>
-        </is>
-      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>6.91</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -1394,12 +1490,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>8.14</t>
+          <t>7.56</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1409,47 +1505,57 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>7.96</t>
+          <t>7.37</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>8.80 7.78 0.52 8.64 7.71 0.54</t>
+          <t>8.80</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>7.19 0.54 8.64 7.12</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
           <t>8.39</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>7.61</t>
-        </is>
-      </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>7.01</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
           <t>7.97</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>7.44</t>
-        </is>
-      </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>6.84</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -1469,12 +1575,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>8.72</t>
+          <t>8.04</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1484,47 +1590,57 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>8.56</t>
+          <t>7.87</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>9.22 8.39 0.53 9.05 8.33 0.54</t>
+          <t>9.22</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>7.70 0.55 9.05 7.63</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>8.80</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>8.23</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>7.53</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
           <t>8.38</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>8.07</t>
-        </is>
-      </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>7.37</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -1544,12 +1660,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>9.37</t>
+          <t>8.58</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1559,47 +1675,57 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>9.22</t>
+          <t>8.42</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>9.43 9.06 0.53 9.26 9.00 0.54</t>
+          <t>9.43</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>8.26 0.55 9.26 8.19</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>9.01</t>
+          <t>0.56</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>8.90</t>
+          <t>9.00</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>8.10</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
           <t>8.59</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>8.75</t>
-        </is>
-      </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>7.94</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0.60</t>
         </is>
       </c>
     </row>
@@ -1619,12 +1745,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>9.11</t>
+          <t>8.32</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1634,47 +1760,57 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>8.97</t>
+          <t>8.18</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10.05 8.83 0.53 9.88 8.78 0.55</t>
+          <t>10.05</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>8.03 0.55 9.88 7.98</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>9.63</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>8.70</t>
-        </is>
-      </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>7.89</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>9.21</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>8.56</t>
-        </is>
-      </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>7.75</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>0.60</t>
         </is>
       </c>
     </row>
@@ -1694,12 +1830,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>8.93</t>
+          <t>8.14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.47</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1709,47 +1845,57 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8.81</t>
+          <t>8.01</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.51</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>10.46 8.68 0.53 10.30 8.63 0.55</t>
+          <t>10.46</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>7.88 0.55 10.30 7.83</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t>10.05</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>8.56</t>
-        </is>
-      </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>7.75</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
           <t>9.63</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>8.43</t>
-        </is>
-      </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>7.62</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0.60</t>
         </is>
       </c>
     </row>
@@ -1764,7 +1910,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1794,6 +1940,27 @@
       <c r="H1" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1804,9 +1971,9 @@
           <t>INDOOR</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>OUTDOOR TEMPERATURE (°CWB)</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>OUTDOOR TEMPERATURE(°CWB)</t>
         </is>
       </c>
     </row>
@@ -1819,20 +1986,26 @@
           <t>EDB</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-10.0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-5.0 0 6.1</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>10.0</t>
-        </is>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>–15</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>–10</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>–5 0</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>6</v>
+      </c>
+      <c r="N3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -1846,20 +2019,45 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TC PI</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>TC PI TC PI TC PI</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>TC</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>TC</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>TC PI TC PI</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>TC</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>TC</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
@@ -1876,22 +2074,47 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2.39 0.66</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2.79 0.69 3.19 0.72 3.67 0.76</t>
+          <t>1.68</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2.01</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3.98</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>0.78</t>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2.35 0.56 3.16 0.73</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>3.64</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.77</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3.96</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.80</t>
         </is>
       </c>
     </row>
@@ -1906,22 +2129,47 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2.25 0.68</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2.65 0.71 3.04 0.74 3.52 0.78</t>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1.91</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2.25 0.57 3.04 0.75</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>3.52</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.79</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>3.84</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0.81</t>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0.82</t>
         </is>
       </c>
     </row>
@@ -1936,22 +2184,47 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2.22 0.68</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2.62 0.71 3.02 0.74 3.50 0.78</t>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1.87</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3.81</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>0.81</t>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2.21 0.58 2.99 0.76</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>3.47</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.82</t>
         </is>
       </c>
     </row>
@@ -1966,22 +2239,47 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2.18 0.69</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2.57 0.72 2.97 0.75 3.45 0.79</t>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1.83</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3.77</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>0.82</t>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2.17 0.59 2.95 0.77</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>3.42</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>3.74</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.83</t>
         </is>
       </c>
     </row>
@@ -1996,22 +2294,47 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2.15 0.69</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2.55 0.72 2.95 0.76 3.42 0.79</t>
+          <t>1.47</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1.81</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>3.74</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>0.82</t>
+          <t>0.56</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2.15 0.59 2.92 0.77</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>3.40</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>3.72</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.83</t>
         </is>
       </c>
     </row>
@@ -2026,22 +2349,47 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.10 0.70</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2.50 0.73 2.90 0.76 3.37 0.80</t>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1.77</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3.69</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0.83</t>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2.10 0.59 2.87 0.78</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>3.35</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.84</t>
         </is>
       </c>
     </row>
@@ -2056,7 +2404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2089,6 +2437,24 @@
       <c r="I1" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2102,14 +2468,20 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>OUTDOOR TEMPERATURE (°FWB)</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>OUTDOOR TEMPERATURE (°FWB)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2121,24 +2493,30 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>14.0</t>
-        </is>
+      <c r="D3" t="n">
+        <v>5</v>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>23.0 32.0 43.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>14</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>50.0</t>
-        </is>
-      </c>
+          <t>23 32</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>43</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="n">
+        <v>50</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2154,24 +2532,42 @@
           <t>TC</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TC PI TC PI TC PI</t>
+          <t>TC</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>TC PI TC PI TC</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PI</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>TC</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
         <is>
           <t>PI</t>
         </is>
@@ -2188,29 +2584,47 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8.15</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.66</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>5.72</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>9.52 0.69 10.88 0.72 12.52 0.76</t>
+          <t>6.87</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>13.58</t>
+          <t>0.53</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.78</t>
+          <t>8.03 0.56 10.80 0.73 12.42</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.77</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>13.51</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>0.80</t>
         </is>
       </c>
     </row>
@@ -2225,29 +2639,47 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7.67</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.68</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>5.37</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9.03 0.71 10.38 0.74 12.01 0.78</t>
+          <t>6.52</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
+          <t>0.55</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>7.67 0.57 10.38 0.75 12.00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.79</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>13.10</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.81</t>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0.82</t>
         </is>
       </c>
     </row>
@@ -2262,29 +2694,47 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.57</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0.68</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>5.23</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>8.94 0.71 10.30 0.74 11.94 0.78</t>
+          <t>6.38</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>13.00</t>
+          <t>0.55</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.81</t>
+          <t>7.53 0.58 10.22 0.76 11.84</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>12.93</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>0.82</t>
         </is>
       </c>
     </row>
@@ -2299,29 +2749,47 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7.44</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0.69</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>5.09</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>8.77 0.72 10.13 0.75 11.77 0.79</t>
+          <t>6.24</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>12.86</t>
+          <t>0.56</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.82</t>
+          <t>7.39 0.59 10.05 0.77 11.68</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>12.76</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>0.83</t>
         </is>
       </c>
     </row>
@@ -2336,29 +2804,47 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7.34</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0.69</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>5.01</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>8.70 0.72 10.07 0.76 11.67 0.79</t>
+          <t>6.17</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>12.76</t>
+          <t>0.56</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.82</t>
+          <t>7.32 0.59 9.97 0.77 11.60</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>12.68</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0.83</t>
         </is>
       </c>
     </row>
@@ -2373,29 +2859,47 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7.17</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0.70</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>4.87</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>8.53 0.73 9.89 0.76 11.50 0.80</t>
+          <t>6.03</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>12.59</t>
+          <t>0.57</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.83</t>
+          <t>7.18 0.59 9.80 0.78 11.43</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>12.51</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0.84</t>
         </is>
       </c>
     </row>

</xml_diff>